<commit_message>
Todo correcto y resultados de 2 ejecuciones
</commit_message>
<xml_diff>
--- a/resources/SistemasVehiculos.xlsx
+++ b/resources/SistemasVehiculos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\profesor\Downloads\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="736">
   <si>
     <t>Nombre</t>
   </si>
@@ -1745,12 +1745,502 @@
   </si>
   <si>
     <t>M7</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>CGM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>GMM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>CSN00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>ALO00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>GMM01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>21508149175421346497</t>
+  </si>
+  <si>
+    <t>21346154503164978451</t>
+  </si>
+  <si>
+    <t>25187786311225455548</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>SFP00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ELR00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>DLR00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>FI5024587946032003165464</t>
+  </si>
+  <si>
+    <t>HAR00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>SPR00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>GPR00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>SAS00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>BFS00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>DFG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>GMG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>MLG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>IAG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09770039F</t>
+  </si>
+  <si>
+    <t>09774199G</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>APM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>GMM02@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ALM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>LDM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>ADG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>LRF00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>LCG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>SBG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>AFG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>DGG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>ROG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>SOG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>VVG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>VMG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>MBG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>CBG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>MSH00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>FDL00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09798076F</t>
+  </si>
+  <si>
+    <t>63516541828944000984</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>SDM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09798287B</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>EGM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09799247M</t>
+  </si>
+  <si>
+    <t>32658012367712548745</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>GPM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09800420M</t>
+  </si>
+  <si>
+    <t>23652365142254222000</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>EAM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09800921T</t>
+  </si>
+  <si>
+    <t>20012541150023365233</t>
+  </si>
+  <si>
+    <t>FR3820012541150023365233</t>
+  </si>
+  <si>
+    <t>MMM00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>09801107W</t>
+  </si>
+  <si>
+    <t>32584216971684051000</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>MGF00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>JAC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>BDC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>NGC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>MLC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>MHG00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>MLC01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>CFC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>CGC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>AT3285550564726165145610</t>
+  </si>
+  <si>
+    <t>HSC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>KSC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
+  </si>
+  <si>
+    <t>MHC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>26551681807651415636</t>
+  </si>
+  <si>
+    <t>IT3526551681807651415636</t>
+  </si>
+  <si>
+    <t>CLD00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>99558741836555551120</t>
+  </si>
+  <si>
+    <t>HU2399558741836555551120</t>
+  </si>
+  <si>
+    <t>MFD00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>52198484752100515144</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>FGD00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>GMM03@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11437269J</t>
+  </si>
+  <si>
+    <t>DK9632541112811220000577</t>
+  </si>
+  <si>
+    <t>IVC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11637421L</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>DMC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11966672W</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>EBC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11662128R</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>NBC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11673213T</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
+    <t>MSC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11942643P</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>MDC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11971207Y</t>
+  </si>
+  <si>
+    <t>ES0421651651812511133547</t>
+  </si>
+  <si>
+    <t>MFC00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11957847D</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>CDD00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11959249P</t>
+  </si>
+  <si>
+    <t>CZ9536250012804785523365</t>
+  </si>
+  <si>
+    <t>CGD00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>11959694Q</t>
+  </si>
+  <si>
+    <t>AT2522515651915640081011</t>
+  </si>
+  <si>
+    <t>HPD00@vehiculos2025.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2129,48 +2619,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="85" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="23.7109375"/>
+    <col min="6" max="6" customWidth="true" style="5" width="7.85546875"/>
+    <col min="7" max="7" customWidth="true" width="85.0"/>
+    <col min="8" max="8" customWidth="true" width="16.140625"/>
+    <col min="10" max="10" customWidth="true" width="22.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -2178,13 +2668,13 @@
       <c r="A2" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2193,16 +2683,22 @@
       <c r="F2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s" s="0">
+        <v>574</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L2">
+      <c r="K2" t="s" s="0">
+        <v>573</v>
+      </c>
+      <c r="L2" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2210,13 +2706,13 @@
       <c r="A3" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -2225,16 +2721,22 @@
       <c r="F3" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s" s="0">
+        <v>576</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>77</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L3">
+      <c r="K3" t="s" s="0">
+        <v>575</v>
+      </c>
+      <c r="L3" s="0">
         <v>25</v>
       </c>
     </row>
@@ -2242,13 +2744,13 @@
       <c r="A4" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2257,16 +2759,22 @@
       <c r="F4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s" s="0">
+        <v>578</v>
+      </c>
+      <c r="H4" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L4">
+      <c r="K4" t="s" s="0">
+        <v>577</v>
+      </c>
+      <c r="L4" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2274,13 +2782,13 @@
       <c r="A5" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>230</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -2289,16 +2797,22 @@
       <c r="F5" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s" s="0">
+        <v>580</v>
+      </c>
+      <c r="H5" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L5">
+      <c r="K5" t="s" s="0">
+        <v>579</v>
+      </c>
+      <c r="L5" s="0">
         <v>50</v>
       </c>
     </row>
@@ -2306,13 +2820,13 @@
       <c r="A6" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -2321,16 +2835,22 @@
       <c r="F6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" t="s" s="0">
+        <v>582</v>
+      </c>
+      <c r="H6" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>78</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L6">
+      <c r="K6" t="s" s="0">
+        <v>581</v>
+      </c>
+      <c r="L6" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2356,13 +2876,13 @@
       <c r="A10" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>228</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -2371,16 +2891,16 @@
       <c r="F10" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>73</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L10">
+        <v>583</v>
+      </c>
+      <c r="L10" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2388,13 +2908,13 @@
       <c r="A11" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" t="s" s="0">
         <v>16</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -2403,16 +2923,16 @@
       <c r="F11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>73</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="L11">
+        <v>584</v>
+      </c>
+      <c r="L11" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2420,13 +2940,13 @@
       <c r="A12" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -2435,16 +2955,16 @@
       <c r="F12" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="L12">
+        <v>585</v>
+      </c>
+      <c r="L12" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2452,13 +2972,13 @@
       <c r="A13" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>234</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="0">
         <v>18</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -2467,16 +2987,22 @@
       <c r="F13" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s" s="0">
+        <v>587</v>
+      </c>
+      <c r="H13" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L13">
+      <c r="K13" t="s" s="0">
+        <v>586</v>
+      </c>
+      <c r="L13" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2484,13 +3010,13 @@
       <c r="A14" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>236</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -2499,16 +3025,22 @@
       <c r="F14" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s" s="0">
+        <v>589</v>
+      </c>
+      <c r="H14" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L14">
+      <c r="K14" t="s" s="0">
+        <v>588</v>
+      </c>
+      <c r="L14" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2516,13 +3048,13 @@
       <c r="A15" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -2531,16 +3063,22 @@
       <c r="F15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s" s="0">
+        <v>591</v>
+      </c>
+      <c r="H15" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L15">
+      <c r="K15" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="L15" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2548,13 +3086,13 @@
       <c r="A16" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -2563,16 +3101,22 @@
       <c r="F16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>593</v>
+      </c>
+      <c r="H16" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" t="s" s="0">
         <v>75</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L16">
+      <c r="K16" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="L16" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2580,13 +3124,13 @@
       <c r="A17" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>233</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -2595,16 +3139,22 @@
       <c r="F17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s" s="0">
+        <v>595</v>
+      </c>
+      <c r="H17" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L17">
+      <c r="K17" t="s" s="0">
+        <v>594</v>
+      </c>
+      <c r="L17" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2612,13 +3162,13 @@
       <c r="A18" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>233</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -2627,16 +3177,22 @@
       <c r="F18" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s" s="0">
+        <v>597</v>
+      </c>
+      <c r="H18" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L18">
+      <c r="K18" t="s" s="0">
+        <v>596</v>
+      </c>
+      <c r="L18" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2644,13 +3200,13 @@
       <c r="A19" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" t="s" s="0">
         <v>22</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -2659,16 +3215,22 @@
       <c r="F19" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s" s="0">
+        <v>599</v>
+      </c>
+      <c r="H19" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L19">
+      <c r="K19" t="s" s="0">
+        <v>598</v>
+      </c>
+      <c r="L19" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2676,13 +3238,13 @@
       <c r="A20" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="0">
         <v>23</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -2691,16 +3253,22 @@
       <c r="F20" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s" s="0">
+        <v>601</v>
+      </c>
+      <c r="H20" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L20">
+      <c r="K20" t="s" s="0">
+        <v>600</v>
+      </c>
+      <c r="L20" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2708,13 +3276,13 @@
       <c r="A21" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" t="s" s="0">
         <v>24</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -2723,16 +3291,22 @@
       <c r="F21" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s" s="0">
+        <v>603</v>
+      </c>
+      <c r="H21" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L21">
+      <c r="K21" t="s" s="0">
+        <v>602</v>
+      </c>
+      <c r="L21" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2740,13 +3314,13 @@
       <c r="A22" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>229</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -2755,16 +3329,22 @@
       <c r="F22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s" s="0">
+        <v>605</v>
+      </c>
+      <c r="H22" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" t="s" s="0">
         <v>79</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L22">
+      <c r="K22" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="L22" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2772,13 +3352,13 @@
       <c r="A23" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>25</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -2787,16 +3367,22 @@
       <c r="F23" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s" s="0">
+        <v>607</v>
+      </c>
+      <c r="H23" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="s" s="0">
         <v>73</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L23">
+      <c r="K23" t="s" s="0">
+        <v>606</v>
+      </c>
+      <c r="L23" s="0">
         <v>0</v>
       </c>
     </row>
@@ -2804,13 +3390,13 @@
       <c r="A24" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" t="s" s="0">
         <v>26</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -2819,30 +3405,36 @@
       <c r="F24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s" s="0">
+        <v>609</v>
+      </c>
+      <c r="H24" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" t="s" s="0">
         <v>73</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="L24">
+      <c r="K24" t="s" s="0">
+        <v>608</v>
+      </c>
+      <c r="L24" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="B25" t="s">
+        <v>276</v>
+      </c>
+      <c r="B25" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>26</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -2851,30 +3443,30 @@
       <c r="F25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B26" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -2883,30 +3475,30 @@
       <c r="F26" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" t="s" s="0">
         <v>76</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="B27" t="s">
+        <v>610</v>
+      </c>
+      <c r="B27" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" t="s" s="0">
         <v>231</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -2915,30 +3507,30 @@
       <c r="F27" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="B28" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" t="s" s="0">
         <v>11</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -2947,30 +3539,30 @@
       <c r="F28" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" t="s" s="0">
         <v>74</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="B29" t="s">
+        <v>611</v>
+      </c>
+      <c r="B29" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" t="s" s="0">
         <v>11</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -2979,16 +3571,16 @@
       <c r="F29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" t="s" s="0">
         <v>79</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3008,13 +3600,13 @@
       <c r="A32" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>281</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>282</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>283</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -3023,16 +3615,22 @@
       <c r="F32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G32" t="s" s="0">
+        <v>613</v>
+      </c>
+      <c r="H32" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="L32">
+      <c r="K32" t="s" s="0">
+        <v>612</v>
+      </c>
+      <c r="L32" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3040,13 +3638,13 @@
       <c r="A33" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>287</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" t="s" s="0">
         <v>288</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -3055,16 +3653,22 @@
       <c r="F33" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s" s="0">
+        <v>615</v>
+      </c>
+      <c r="H33" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" t="s" s="0">
         <v>79</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="L33">
+      <c r="K33" t="s" s="0">
+        <v>614</v>
+      </c>
+      <c r="L33" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3072,13 +3676,13 @@
       <c r="A34" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>293</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -3087,16 +3691,22 @@
       <c r="F34" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s" s="0">
+        <v>617</v>
+      </c>
+      <c r="H34" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="L34">
+      <c r="K34" t="s" s="0">
+        <v>616</v>
+      </c>
+      <c r="L34" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3104,13 +3714,13 @@
       <c r="A35" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>296</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>297</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" t="s" s="0">
         <v>298</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -3119,16 +3729,22 @@
       <c r="F35" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="H35" t="s">
+      <c r="G35" t="s" s="0">
+        <v>619</v>
+      </c>
+      <c r="H35" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="L35">
+      <c r="K35" t="s" s="0">
+        <v>618</v>
+      </c>
+      <c r="L35" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3136,13 +3752,13 @@
       <c r="A36" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" t="s" s="0">
         <v>304</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -3151,16 +3767,22 @@
       <c r="F36" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H36" t="s">
+      <c r="G36" t="s" s="0">
+        <v>621</v>
+      </c>
+      <c r="H36" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="L36">
+      <c r="K36" t="s" s="0">
+        <v>620</v>
+      </c>
+      <c r="L36" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3168,13 +3790,13 @@
       <c r="A37" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>307</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" t="s" s="0">
         <v>308</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -3183,16 +3805,22 @@
       <c r="F37" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="H37" t="s">
+      <c r="G37" t="s" s="0">
+        <v>623</v>
+      </c>
+      <c r="H37" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="L37">
+      <c r="K37" t="s" s="0">
+        <v>622</v>
+      </c>
+      <c r="L37" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3200,13 +3828,13 @@
       <c r="A38" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>312</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>313</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -3215,16 +3843,22 @@
       <c r="F38" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H38" t="s">
+      <c r="G38" t="s" s="0">
+        <v>625</v>
+      </c>
+      <c r="H38" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="L38">
+      <c r="K38" t="s" s="0">
+        <v>624</v>
+      </c>
+      <c r="L38" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3232,13 +3866,13 @@
       <c r="A39" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" t="s" s="0">
         <v>318</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -3247,16 +3881,22 @@
       <c r="F39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39" t="s" s="0">
+        <v>627</v>
+      </c>
+      <c r="H39" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="L39">
+      <c r="K39" t="s" s="0">
+        <v>626</v>
+      </c>
+      <c r="L39" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3264,13 +3904,13 @@
       <c r="A40" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" t="s" s="0">
         <v>321</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -3279,16 +3919,22 @@
       <c r="F40" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="H40" t="s">
+      <c r="G40" t="s" s="0">
+        <v>629</v>
+      </c>
+      <c r="H40" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L40">
+      <c r="K40" t="s" s="0">
+        <v>628</v>
+      </c>
+      <c r="L40" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3296,13 +3942,13 @@
       <c r="A41" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" t="s" s="0">
         <v>324</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -3311,16 +3957,22 @@
       <c r="F41" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="H41" t="s">
+      <c r="G41" t="s" s="0">
+        <v>631</v>
+      </c>
+      <c r="H41" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="L41">
+      <c r="K41" t="s" s="0">
+        <v>630</v>
+      </c>
+      <c r="L41" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3328,13 +3980,13 @@
       <c r="A42" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>329</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -3343,16 +3995,22 @@
       <c r="F42" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" t="s" s="0">
+        <v>633</v>
+      </c>
+      <c r="H42" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="L42">
+      <c r="K42" t="s" s="0">
+        <v>632</v>
+      </c>
+      <c r="L42" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3360,13 +4018,13 @@
       <c r="A43" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="s" s="0">
         <v>328</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" t="s" s="0">
         <v>333</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -3375,16 +4033,22 @@
       <c r="F43" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H43" t="s">
+      <c r="G43" t="s" s="0">
+        <v>634</v>
+      </c>
+      <c r="H43" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="L43">
+      <c r="K43" t="s" s="0">
+        <v>612</v>
+      </c>
+      <c r="L43" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3392,13 +4056,13 @@
       <c r="A44" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" t="s" s="0">
         <v>336</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -3407,16 +4071,22 @@
       <c r="F44" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G44" t="s" s="0">
+        <v>636</v>
+      </c>
+      <c r="H44" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" t="s" s="0">
         <v>77</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="L44">
+      <c r="K44" t="s" s="0">
+        <v>635</v>
+      </c>
+      <c r="L44" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3424,13 +4094,13 @@
       <c r="A45" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="s" s="0">
         <v>339</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="s" s="0">
         <v>336</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -3439,16 +4109,22 @@
       <c r="F45" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="H45" t="s">
+      <c r="G45" t="s" s="0">
+        <v>638</v>
+      </c>
+      <c r="H45" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J45" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="L45">
+      <c r="K45" t="s" s="0">
+        <v>637</v>
+      </c>
+      <c r="L45" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3456,13 +4132,13 @@
       <c r="A46" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="s" s="0">
         <v>342</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>343</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -3471,16 +4147,22 @@
       <c r="F46" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G46" t="s" s="0">
+        <v>640</v>
+      </c>
+      <c r="H46" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="L46">
+      <c r="K46" t="s" s="0">
+        <v>639</v>
+      </c>
+      <c r="L46" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3488,13 +4170,13 @@
       <c r="A47" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>348</v>
       </c>
       <c r="E47" s="4" t="s">
@@ -3503,16 +4185,22 @@
       <c r="F47" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H47" t="s">
+      <c r="G47" t="s" s="0">
+        <v>642</v>
+      </c>
+      <c r="H47" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="L47">
+      <c r="K47" t="s" s="0">
+        <v>641</v>
+      </c>
+      <c r="L47" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3520,13 +4208,13 @@
       <c r="A48" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>352</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" t="s" s="0">
         <v>353</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -3535,16 +4223,22 @@
       <c r="F48" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H48" t="s">
+      <c r="G48" t="s" s="0">
+        <v>644</v>
+      </c>
+      <c r="H48" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" t="s" s="0">
         <v>354</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="L48">
+      <c r="K48" t="s" s="0">
+        <v>643</v>
+      </c>
+      <c r="L48" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3552,13 +4246,13 @@
       <c r="A49" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>358</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" t="s" s="0">
         <v>359</v>
       </c>
       <c r="E49" s="4" t="s">
@@ -3567,16 +4261,22 @@
       <c r="F49" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H49" t="s">
+      <c r="G49" t="s" s="0">
+        <v>646</v>
+      </c>
+      <c r="H49" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="L49">
+      <c r="K49" t="s" s="0">
+        <v>645</v>
+      </c>
+      <c r="L49" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3588,15 +4288,15 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="B51" t="s">
+        <v>647</v>
+      </c>
+      <c r="B51" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>363</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" t="s" s="0">
         <v>364</v>
       </c>
       <c r="E51" s="4" t="s">
@@ -3605,30 +4305,36 @@
       <c r="F51" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H51" t="s">
+      <c r="G51" t="s" s="0">
+        <v>650</v>
+      </c>
+      <c r="H51" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="L51">
+        <v>648</v>
+      </c>
+      <c r="K51" t="s" s="0">
+        <v>649</v>
+      </c>
+      <c r="L51" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="B52" t="s">
+        <v>651</v>
+      </c>
+      <c r="B52" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>282</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>367</v>
       </c>
       <c r="E52" s="4" t="s">
@@ -3637,30 +4343,36 @@
       <c r="F52" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="H52" t="s">
+      <c r="G52" t="s" s="0">
+        <v>654</v>
+      </c>
+      <c r="H52" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="L52">
+        <v>652</v>
+      </c>
+      <c r="K52" t="s" s="0">
+        <v>653</v>
+      </c>
+      <c r="L52" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="B53" t="s">
+        <v>655</v>
+      </c>
+      <c r="B53" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" t="s" s="0">
         <v>371</v>
       </c>
       <c r="E53" s="4" t="s">
@@ -3669,30 +4381,36 @@
       <c r="F53" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H53" t="s">
+      <c r="G53" t="s" s="0">
+        <v>658</v>
+      </c>
+      <c r="H53" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" t="s" s="0">
         <v>75</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="L53">
+        <v>656</v>
+      </c>
+      <c r="K53" t="s" s="0">
+        <v>657</v>
+      </c>
+      <c r="L53" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="B54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B54" t="s" s="0">
         <v>375</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>376</v>
       </c>
       <c r="E54" s="4" t="s">
@@ -3701,30 +4419,36 @@
       <c r="F54" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="H54" t="s">
+      <c r="G54" t="s" s="0">
+        <v>662</v>
+      </c>
+      <c r="H54" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="L54">
+        <v>660</v>
+      </c>
+      <c r="K54" t="s" s="0">
+        <v>661</v>
+      </c>
+      <c r="L54" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="B55" t="s">
+        <v>663</v>
+      </c>
+      <c r="B55" t="s" s="0">
         <v>381</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>297</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="0">
         <v>382</v>
       </c>
       <c r="E55" s="4" t="s">
@@ -3733,30 +4457,36 @@
       <c r="F55" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H55" t="s">
+      <c r="G55" t="s" s="0">
+        <v>666</v>
+      </c>
+      <c r="H55" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" t="s" s="0">
         <v>78</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="L55">
+        <v>664</v>
+      </c>
+      <c r="K55" t="s" s="0">
+        <v>665</v>
+      </c>
+      <c r="L55" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B56" t="s">
+        <v>667</v>
+      </c>
+      <c r="B56" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" t="s" s="0">
         <v>385</v>
       </c>
       <c r="E56" s="4" t="s">
@@ -3765,16 +4495,22 @@
       <c r="F56" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="H56" t="s">
+      <c r="G56" t="s" s="0">
+        <v>670</v>
+      </c>
+      <c r="H56" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="L56">
+        <v>668</v>
+      </c>
+      <c r="K56" t="s" s="0">
+        <v>669</v>
+      </c>
+      <c r="L56" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3788,13 +4524,13 @@
       <c r="A58" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>390</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>391</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -3803,16 +4539,22 @@
       <c r="F58" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H58" t="s">
+      <c r="G58" t="s" s="0">
+        <v>672</v>
+      </c>
+      <c r="H58" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="L58">
+      <c r="K58" t="s" s="0">
+        <v>671</v>
+      </c>
+      <c r="L58" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3820,13 +4562,13 @@
       <c r="A59" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>303</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>395</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" t="s" s="0">
         <v>396</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -3835,16 +4577,22 @@
       <c r="F59" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H59" t="s">
+      <c r="G59" t="s" s="0">
+        <v>674</v>
+      </c>
+      <c r="H59" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" t="s" s="0">
         <v>397</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="L59">
+      <c r="K59" t="s" s="0">
+        <v>673</v>
+      </c>
+      <c r="L59" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3852,13 +4600,13 @@
       <c r="A60" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>400</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>401</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -3867,16 +4615,22 @@
       <c r="F60" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="H60" t="s">
+      <c r="G60" t="s" s="0">
+        <v>676</v>
+      </c>
+      <c r="H60" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="L60">
+      <c r="K60" t="s" s="0">
+        <v>675</v>
+      </c>
+      <c r="L60" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3884,13 +4638,13 @@
       <c r="A61" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>405</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>406</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>407</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -3899,16 +4653,22 @@
       <c r="F61" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="H61" t="s">
+      <c r="G61" t="s" s="0">
+        <v>678</v>
+      </c>
+      <c r="H61" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="L61">
+      <c r="K61" t="s" s="0">
+        <v>677</v>
+      </c>
+      <c r="L61" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3916,13 +4676,13 @@
       <c r="A62" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>25</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -3931,16 +4691,22 @@
       <c r="F62" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="H62" t="s">
+      <c r="G62" t="s" s="0">
+        <v>680</v>
+      </c>
+      <c r="H62" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" t="s" s="0">
         <v>76</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="L62">
+      <c r="K62" t="s" s="0">
+        <v>679</v>
+      </c>
+      <c r="L62" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3948,13 +4714,13 @@
       <c r="A63" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>415</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>416</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -3963,16 +4729,22 @@
       <c r="F63" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H63" t="s">
+      <c r="G63" t="s" s="0">
+        <v>682</v>
+      </c>
+      <c r="H63" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" t="s" s="0">
         <v>418</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="L63">
+      <c r="K63" t="s" s="0">
+        <v>681</v>
+      </c>
+      <c r="L63" s="0">
         <v>0</v>
       </c>
     </row>
@@ -3980,13 +4752,13 @@
       <c r="A64" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>421</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" t="s" s="0">
         <v>422</v>
       </c>
       <c r="E64" s="4" t="s">
@@ -3995,16 +4767,22 @@
       <c r="F64" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="H64" t="s">
+      <c r="G64" t="s" s="0">
+        <v>684</v>
+      </c>
+      <c r="H64" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="L64">
+      <c r="K64" t="s" s="0">
+        <v>683</v>
+      </c>
+      <c r="L64" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4012,13 +4790,13 @@
       <c r="A65" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>428</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" t="s" s="0">
         <v>429</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -4027,16 +4805,22 @@
       <c r="F65" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="H65" t="s">
+      <c r="G65" t="s" s="0">
+        <v>686</v>
+      </c>
+      <c r="H65" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="L65">
+      <c r="K65" t="s" s="0">
+        <v>685</v>
+      </c>
+      <c r="L65" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4044,13 +4828,13 @@
       <c r="A66" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" t="s" s="0">
         <v>433</v>
       </c>
       <c r="E66" s="4" t="s">
@@ -4059,16 +4843,22 @@
       <c r="F66" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="H66" t="s">
+      <c r="G66" t="s" s="0">
+        <v>688</v>
+      </c>
+      <c r="H66" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" t="s" s="0">
         <v>436</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="L66">
+      <c r="K66" t="s" s="0">
+        <v>687</v>
+      </c>
+      <c r="L66" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4076,13 +4866,13 @@
       <c r="A67" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>439</v>
       </c>
       <c r="E67" s="4" t="s">
@@ -4091,16 +4881,22 @@
       <c r="F67" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="H67" t="s">
+      <c r="G67" t="s" s="0">
+        <v>690</v>
+      </c>
+      <c r="H67" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="L67">
+      <c r="K67" t="s" s="0">
+        <v>689</v>
+      </c>
+      <c r="L67" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4143,13 +4939,13 @@
       <c r="A74" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" t="s" s="0">
         <v>410</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" t="s" s="0">
         <v>444</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" t="s" s="0">
         <v>343</v>
       </c>
       <c r="E74" s="4" t="s">
@@ -4158,16 +4954,22 @@
       <c r="F74" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="H74" t="s">
+      <c r="G74" t="s" s="0">
+        <v>693</v>
+      </c>
+      <c r="H74" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" t="s" s="0">
         <v>436</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="L74">
+        <v>691</v>
+      </c>
+      <c r="K74" t="s" s="0">
+        <v>692</v>
+      </c>
+      <c r="L74" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4175,13 +4977,13 @@
       <c r="A75" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" t="s" s="0">
         <v>235</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" t="s" s="0">
         <v>448</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" t="s" s="0">
         <v>348</v>
       </c>
       <c r="E75" s="4" t="s">
@@ -4190,16 +4992,22 @@
       <c r="F75" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="H75" t="s">
+      <c r="G75" t="s" s="0">
+        <v>696</v>
+      </c>
+      <c r="H75" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" t="s" s="0">
         <v>451</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="L75">
+        <v>694</v>
+      </c>
+      <c r="K75" t="s" s="0">
+        <v>695</v>
+      </c>
+      <c r="L75" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4207,13 +5015,13 @@
       <c r="A76" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>454</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" t="s" s="0">
         <v>353</v>
       </c>
       <c r="E76" s="4" t="s">
@@ -4222,16 +5030,22 @@
       <c r="F76" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H76" t="s">
+      <c r="G76" t="s" s="0">
+        <v>699</v>
+      </c>
+      <c r="H76" t="s" s="0">
         <v>565</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" t="s" s="0">
         <v>456</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="L76">
+        <v>697</v>
+      </c>
+      <c r="K76" t="s" s="0">
+        <v>698</v>
+      </c>
+      <c r="L76" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4239,13 +5053,13 @@
       <c r="A77" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" t="s" s="0">
         <v>427</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" t="s" s="0">
         <v>359</v>
       </c>
       <c r="E77" s="4" t="s">
@@ -4254,16 +5068,22 @@
       <c r="F77" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H77" t="s">
+      <c r="G77" t="s" s="0">
+        <v>702</v>
+      </c>
+      <c r="H77" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="L77">
+        <v>700</v>
+      </c>
+      <c r="K77" t="s" s="0">
+        <v>701</v>
+      </c>
+      <c r="L77" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4271,13 +5091,13 @@
       <c r="A78" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E78" s="4" t="s">
@@ -4286,16 +5106,22 @@
       <c r="F78" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H78" t="s">
+      <c r="G78" t="s" s="0">
+        <v>705</v>
+      </c>
+      <c r="H78" t="s" s="0">
         <v>275</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" t="s" s="0">
         <v>462</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="L78">
+        <v>703</v>
+      </c>
+      <c r="K78" t="s" s="0">
+        <v>704</v>
+      </c>
+      <c r="L78" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4401,15 +5227,15 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="B99" t="s">
+        <v>706</v>
+      </c>
+      <c r="B99" t="s" s="0">
         <v>335</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" t="s" s="0">
         <v>465</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" t="s" s="0">
         <v>466</v>
       </c>
       <c r="E99" s="4" t="s">
@@ -4418,30 +5244,36 @@
       <c r="F99" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="H99" t="s">
+      <c r="G99" t="s" s="0">
+        <v>708</v>
+      </c>
+      <c r="H99" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" t="s" s="0">
         <v>469</v>
       </c>
       <c r="J99" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="L99">
+      <c r="K99" t="s" s="0">
+        <v>707</v>
+      </c>
+      <c r="L99" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="B100" t="s">
+        <v>709</v>
+      </c>
+      <c r="B100" t="s" s="0">
         <v>339</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" t="s" s="0">
         <v>472</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" t="s" s="0">
         <v>473</v>
       </c>
       <c r="E100" s="4" t="s">
@@ -4450,30 +5282,36 @@
       <c r="F100" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="H100" t="s">
+      <c r="G100" t="s" s="0">
+        <v>711</v>
+      </c>
+      <c r="H100" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" t="s" s="0">
         <v>397</v>
       </c>
       <c r="J100" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="L100">
+      <c r="K100" t="s" s="0">
+        <v>710</v>
+      </c>
+      <c r="L100" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="B101" t="s">
+        <v>712</v>
+      </c>
+      <c r="B101" t="s" s="0">
         <v>342</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" t="s" s="0">
         <v>478</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" t="s" s="0">
         <v>479</v>
       </c>
       <c r="E101" s="4" t="s">
@@ -4482,30 +5320,36 @@
       <c r="F101" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="H101" t="s">
+      <c r="G101" t="s" s="0">
+        <v>714</v>
+      </c>
+      <c r="H101" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="L101">
+      <c r="K101" t="s" s="0">
+        <v>713</v>
+      </c>
+      <c r="L101" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>482</v>
-      </c>
-      <c r="B102" t="s">
+        <v>715</v>
+      </c>
+      <c r="B102" t="s" s="0">
         <v>317</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" t="s" s="0">
         <v>483</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" t="s" s="0">
         <v>401</v>
       </c>
       <c r="E102" s="4" t="s">
@@ -4514,30 +5358,36 @@
       <c r="F102" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="H102" t="s">
+      <c r="G102" t="s" s="0">
+        <v>717</v>
+      </c>
+      <c r="H102" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="L102">
+      <c r="K102" t="s" s="0">
+        <v>716</v>
+      </c>
+      <c r="L102" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="B103" t="s">
+        <v>718</v>
+      </c>
+      <c r="B103" t="s" s="0">
         <v>351</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" t="s" s="0">
         <v>486</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" t="s" s="0">
         <v>407</v>
       </c>
       <c r="E103" s="4" t="s">
@@ -4546,30 +5396,36 @@
       <c r="F103" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="H103" t="s">
+      <c r="G103" t="s" s="0">
+        <v>720</v>
+      </c>
+      <c r="H103" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="L103">
+      <c r="K103" t="s" s="0">
+        <v>719</v>
+      </c>
+      <c r="L103" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="B104" t="s">
+        <v>721</v>
+      </c>
+      <c r="B104" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" t="s" s="0">
         <v>490</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" t="s" s="0">
         <v>25</v>
       </c>
       <c r="E104" s="4" t="s">
@@ -4578,30 +5434,36 @@
       <c r="F104" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="H104" t="s">
+      <c r="G104" t="s" s="0">
+        <v>723</v>
+      </c>
+      <c r="H104" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J104" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="L104">
+      <c r="K104" t="s" s="0">
+        <v>722</v>
+      </c>
+      <c r="L104" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>492</v>
-      </c>
-      <c r="B105" t="s">
+        <v>724</v>
+      </c>
+      <c r="B105" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" t="s" s="0">
         <v>444</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" t="s" s="0">
         <v>416</v>
       </c>
       <c r="E105" s="4" t="s">
@@ -4610,30 +5472,36 @@
       <c r="F105" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="H105" t="s">
+      <c r="G105" t="s" s="0">
+        <v>726</v>
+      </c>
+      <c r="H105" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="L105">
+      <c r="K105" t="s" s="0">
+        <v>725</v>
+      </c>
+      <c r="L105" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>495</v>
-      </c>
-      <c r="B106" t="s">
+        <v>727</v>
+      </c>
+      <c r="B106" t="s" s="0">
         <v>362</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" t="s" s="0">
         <v>448</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" t="s" s="0">
         <v>422</v>
       </c>
       <c r="E106" s="4" t="s">
@@ -4642,30 +5510,36 @@
       <c r="F106" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="H106" t="s">
+      <c r="G106" t="s" s="0">
+        <v>729</v>
+      </c>
+      <c r="H106" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106" t="s" s="0">
         <v>72</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="L106">
+      <c r="K106" t="s" s="0">
+        <v>728</v>
+      </c>
+      <c r="L106" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="B107" t="s">
+        <v>730</v>
+      </c>
+      <c r="B107" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" t="s" s="0">
         <v>454</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" t="s" s="0">
         <v>429</v>
       </c>
       <c r="E107" s="4" t="s">
@@ -4674,30 +5548,36 @@
       <c r="F107" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="H107" t="s">
+      <c r="G107" t="s" s="0">
+        <v>732</v>
+      </c>
+      <c r="H107" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107" t="s" s="0">
         <v>500</v>
       </c>
       <c r="J107" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="L107">
+      <c r="K107" t="s" s="0">
+        <v>731</v>
+      </c>
+      <c r="L107" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="B108" t="s">
+        <v>733</v>
+      </c>
+      <c r="B108" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" t="s" s="0">
         <v>357</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" t="s" s="0">
         <v>433</v>
       </c>
       <c r="E108" s="4" t="s">
@@ -4706,16 +5586,22 @@
       <c r="F108" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H108" t="s">
+      <c r="G108" t="s" s="0">
+        <v>735</v>
+      </c>
+      <c r="H108" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I108" t="s" s="0">
         <v>436</v>
       </c>
       <c r="J108" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="L108">
+      <c r="K108" t="s" s="0">
+        <v>734</v>
+      </c>
+      <c r="L108" s="0">
         <v>0</v>
       </c>
     </row>
@@ -4758,19 +5644,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.28515625"/>
+    <col min="2" max="2" customWidth="true" width="17.0"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.42578125"/>
+    <col min="4" max="4" style="1" width="11.42578125"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375"/>
+    <col min="14" max="14" customWidth="true" width="13.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>209</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4779,42 +5665,42 @@
       <c r="D1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>215</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -4830,10 +5716,10 @@
         <v>202</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>900</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K2" s="7">
@@ -4847,10 +5733,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4862,10 +5748,10 @@
       <c r="E3" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>1800</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>279</v>
       </c>
       <c r="K3" s="7">
@@ -4882,10 +5768,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -4897,10 +5783,10 @@
       <c r="E4" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K4" s="7">
@@ -4917,10 +5803,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -4932,10 +5818,10 @@
       <c r="E5" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>14</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K5" s="7">
@@ -4949,7 +5835,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -4965,10 +5851,10 @@
         <v>197</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>900</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K6" s="7">
@@ -4982,7 +5868,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -5000,7 +5886,7 @@
       <c r="F7" s="8">
         <v>11.64</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>279</v>
       </c>
       <c r="K7" s="7">
@@ -5027,7 +5913,7 @@
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -5045,7 +5931,7 @@
       <c r="F9" s="8">
         <v>13.29</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K9" s="7">
@@ -5059,10 +5945,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>114</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -5074,10 +5960,10 @@
       <c r="E10" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>18</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K10" s="7">
@@ -5091,10 +5977,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -5106,10 +5992,10 @@
       <c r="E11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>21</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K11" s="7">
@@ -5123,10 +6009,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>134</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -5138,10 +6024,10 @@
       <c r="E12" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>25</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K12" s="7">
@@ -5162,10 +6048,10 @@
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>125</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -5177,10 +6063,10 @@
       <c r="E14" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>15</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K14" s="7">
@@ -5194,10 +6080,10 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -5209,10 +6095,10 @@
       <c r="E15" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>35</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K15" s="7">
@@ -5226,10 +6112,10 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>127</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -5241,10 +6127,10 @@
       <c r="E16" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>65</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K16" s="7">
@@ -5268,10 +6154,10 @@
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -5283,10 +6169,10 @@
       <c r="E18" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="0">
         <v>950</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K18" s="7">
@@ -5300,10 +6186,10 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -5315,10 +6201,10 @@
       <c r="E19" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="0">
         <v>2500</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K19" s="7">
@@ -5332,10 +6218,10 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -5347,10 +6233,10 @@
       <c r="E20" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="0">
         <v>6500</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K20" s="7">
@@ -5364,10 +6250,10 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5379,10 +6265,10 @@
       <c r="E21" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="0">
         <v>12500</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K21" s="7">
@@ -5403,10 +6289,10 @@
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5418,10 +6304,10 @@
       <c r="E23" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>31</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K23" s="7">
@@ -5445,10 +6331,10 @@
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -5460,10 +6346,10 @@
       <c r="E25" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="0">
         <v>850</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K25" s="7">
@@ -5477,10 +6363,10 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>171</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -5492,10 +6378,10 @@
       <c r="E26" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="0">
         <v>3250</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K26" s="7">
@@ -5516,10 +6402,10 @@
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>150</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>121</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -5531,10 +6417,10 @@
       <c r="E28" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="0">
         <v>49</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K28" s="7">
@@ -5555,7 +6441,7 @@
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -5570,10 +6456,10 @@
       <c r="E30" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="0">
         <v>125</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K30" s="7">
@@ -5587,7 +6473,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -5602,10 +6488,10 @@
       <c r="E31" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="0">
         <v>300</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K31" s="7">
@@ -5619,7 +6505,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -5634,10 +6520,10 @@
       <c r="E32" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="0">
         <v>600</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K32" s="7">
@@ -5654,7 +6540,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -5669,10 +6555,10 @@
       <c r="E33" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="0">
         <v>1500</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K33" s="7">
@@ -5706,7 +6592,7 @@
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B39" s="8" t="s">
@@ -5724,7 +6610,7 @@
       <c r="F39" s="8">
         <v>9.0500000000000007</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K39" s="7">
@@ -5738,7 +6624,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -5756,7 +6642,7 @@
       <c r="F40" s="8">
         <v>13.58</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K40" s="7">
@@ -5773,7 +6659,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -5788,10 +6674,10 @@
       <c r="E41" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="0">
         <v>18.21</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K41" s="7">
@@ -5829,7 +6715,7 @@
       <c r="O44" s="8"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -5844,10 +6730,10 @@
       <c r="E45" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="0">
         <v>21.05</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K45" s="7">
@@ -5861,7 +6747,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" t="s" s="0">
         <v>145</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -5876,10 +6762,10 @@
       <c r="E46" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="0">
         <v>26.03</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K46" s="7">
@@ -5909,7 +6795,7 @@
       <c r="O48" s="8"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" t="s" s="0">
         <v>146</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -5924,10 +6810,10 @@
       <c r="E49" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="0">
         <v>15</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K49" s="7">
@@ -5941,7 +6827,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" t="s" s="0">
         <v>146</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -5956,10 +6842,10 @@
       <c r="E50" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="0">
         <v>35</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K50" s="7">
@@ -5973,7 +6859,7 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" t="s" s="0">
         <v>146</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -5988,10 +6874,10 @@
       <c r="E51" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="0">
         <v>65</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K51" s="7">
@@ -6013,7 +6899,7 @@
       <c r="O52" s="8"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" t="s" s="0">
         <v>147</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -6028,10 +6914,10 @@
       <c r="E53" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="0">
         <v>950</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K53" s="7">
@@ -6048,7 +6934,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" t="s" s="0">
         <v>147</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -6063,10 +6949,10 @@
       <c r="E54" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="0">
         <v>2500</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K54" s="7">
@@ -6080,7 +6966,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" t="s" s="0">
         <v>147</v>
       </c>
       <c r="B55" s="8" t="s">
@@ -6095,10 +6981,10 @@
       <c r="E55" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="0">
         <v>6500</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K55" s="7">
@@ -6112,7 +6998,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" t="s" s="0">
         <v>147</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -6127,10 +7013,10 @@
       <c r="E56" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="0">
         <v>12500</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K56" s="7">
@@ -6151,7 +7037,7 @@
       <c r="L57" s="7"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" t="s" s="0">
         <v>148</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -6166,10 +7052,10 @@
       <c r="E58" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="0">
         <v>14</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K58" s="7">
@@ -6183,7 +7069,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" t="s" s="0">
         <v>148</v>
       </c>
       <c r="B59" s="8" t="s">
@@ -6198,10 +7084,10 @@
       <c r="E59" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="0">
         <v>20</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K59" s="7">
@@ -6215,7 +7101,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" t="s" s="0">
         <v>148</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -6230,10 +7116,10 @@
       <c r="E60" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="0">
         <v>31</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K60" s="7">
@@ -6255,7 +7141,7 @@
       <c r="O61" s="1"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" t="s" s="0">
         <v>149</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -6270,10 +7156,10 @@
       <c r="E62" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="0">
         <v>850</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K62" s="7">
@@ -6287,7 +7173,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" t="s" s="0">
         <v>149</v>
       </c>
       <c r="B63" s="8" t="s">
@@ -6302,10 +7188,10 @@
       <c r="E63" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="0">
         <v>1800</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K63" s="7">
@@ -6319,7 +7205,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" t="s" s="0">
         <v>149</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -6334,10 +7220,10 @@
       <c r="E64" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="0">
         <v>3250</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K64" s="7">
@@ -6358,7 +7244,7 @@
       <c r="L65" s="7"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" t="s" s="0">
         <v>150</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -6373,10 +7259,10 @@
       <c r="E66" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="0">
         <v>49</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K66" s="7">
@@ -6398,7 +7284,7 @@
       <c r="O67" s="2"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B68" s="8" t="s">
@@ -6413,10 +7299,10 @@
       <c r="E68" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="0">
         <v>125</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J68" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K68" s="7">
@@ -6430,7 +7316,7 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -6445,10 +7331,10 @@
       <c r="E69" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="0">
         <v>300</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K69" s="7">
@@ -6462,7 +7348,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -6477,10 +7363,10 @@
       <c r="E70" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="0">
         <v>600</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J70" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K70" s="7">
@@ -6494,7 +7380,7 @@
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" t="s" s="0">
         <v>151</v>
       </c>
       <c r="B71" s="8" t="s">
@@ -6509,10 +7395,10 @@
       <c r="E71" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="0">
         <v>1500</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J71" t="s" s="0">
         <v>219</v>
       </c>
       <c r="K71" s="7">

</xml_diff>